<commit_message>
reverted User creation to not allow empty string urls
</commit_message>
<xml_diff>
--- a/tests/Testing_Resources/accounts_to_follow_06.xlsx
+++ b/tests/Testing_Resources/accounts_to_follow_06.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kenan/Library/CloudStorage/OneDrive-Personal/Personal Development/Python/TwitterToolsLibrary/tests/Testing_Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc0eafcf01cf0dc5/Personal Development/Python/TwitterToolsLibrary/tests/Testing_Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FDD6F7-C3C6-C34A-BFFA-613C174A5A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D2FDD6F7-C3C6-C34A-BFFA-613C174A5A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCE847B2-549F-AD4E-81E1-9448462E5689}"/>
   <bookViews>
     <workbookView xWindow="10700" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>handle</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>https://twitter.com/account_6</t>
-  </si>
-  <si>
-    <t>https://twitter.com/</t>
   </si>
 </sst>
 </file>
@@ -488,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -690,8 +687,11 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -700,23 +700,6 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
         <v>20</v>
       </c>
     </row>
@@ -728,12 +711,11 @@
     <hyperlink ref="B5" r:id="rId4" xr:uid="{9FF39D07-FB61-DD4C-BA56-EB9B0FADE0A2}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{E4D0594D-6479-B247-AF76-88815EBB15C2}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{4CE4CB29-8531-3D4D-9DAC-AD0CDF0C3B13}"/>
-    <hyperlink ref="B13" r:id="rId7" xr:uid="{22BDBFEA-BBBA-824F-BFBF-B9B7E0C13BFB}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{22BDBFEA-BBBA-824F-BFBF-B9B7E0C13BFB}"/>
     <hyperlink ref="B8" r:id="rId8" xr:uid="{9C9FFFF9-3A2E-B94E-BD2A-E880D37F9682}"/>
     <hyperlink ref="B9" r:id="rId9" xr:uid="{5C808054-E6AA-1B42-A3EE-B52D7137E9E1}"/>
     <hyperlink ref="B10" r:id="rId10" xr:uid="{17B70278-76D4-4140-B10C-BC9742648DB9}"/>
     <hyperlink ref="B11" r:id="rId11" xr:uid="{B764E37B-3F28-7248-8972-A7DD7CB2CDC8}"/>
-    <hyperlink ref="B12" r:id="rId12" xr:uid="{5E3CE44D-E185-4D45-A644-0DEDCFDB8C4F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>